<commit_message>
- update code git
</commit_message>
<xml_diff>
--- a/src/main/resources/Template1.xlsx
+++ b/src/main/resources/Template1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Log</t>
   </si>
   <si>
-    <t xml:space="preserve">Tester's Name </t>
-  </si>
-  <si>
-    <t>Date Tested</t>
-  </si>
-  <si>
     <t>Test Case Results</t>
   </si>
   <si>
@@ -73,12 +67,30 @@
   </si>
   <si>
     <t>Pass / Fail / Not executed / Suspended</t>
+  </si>
+  <si>
+    <t>Reviewed Date</t>
+  </si>
+  <si>
+    <t>Created Date</t>
+  </si>
+  <si>
+    <t>Date Tested (mm/dd/yy hh:mm:ss)</t>
+  </si>
+  <si>
+    <t>Test Case Location</t>
+  </si>
+  <si>
+    <t>Tester's Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -165,12 +177,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -199,10 +226,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -486,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,109 +553,435 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>1</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- Update default value
</commit_message>
<xml_diff>
--- a/src/main/resources/Template1.xlsx
+++ b/src/main/resources/Template1.xlsx
@@ -48,9 +48,6 @@
     <t>Log</t>
   </si>
   <si>
-    <t>Test Case Results</t>
-  </si>
-  <si>
     <t>Step #</t>
   </si>
   <si>
@@ -78,10 +75,13 @@
     <t>Date Tested (mm/dd/yy hh:mm:ss)</t>
   </si>
   <si>
-    <t>Test Case Location</t>
-  </si>
-  <si>
     <t>Tester's Name</t>
+  </si>
+  <si>
+    <t>Test Case Results (Pass / Fail / Not executed / Suspended)</t>
+  </si>
+  <si>
+    <t>Test Case Script Location</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,17 +567,17 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="1" t="s">
@@ -609,15 +609,15 @@
     </row>
     <row r="7" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F7" s="13"/>
     </row>
@@ -631,22 +631,22 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>